<commit_message>
Added Logan Paul alien hat
</commit_message>
<xml_diff>
--- a/sprites/land/mapDesign.xlsx
+++ b/sprites/land/mapDesign.xlsx
@@ -454,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW98"/>
+  <dimension ref="A1:AY98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P47" sqref="P47"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD29" sqref="AD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1262,7 @@
       <c r="AV16" s="4"/>
       <c r="AW16" s="4"/>
     </row>
-    <row r="17" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="8"/>
@@ -1280,7 +1280,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1297,40 +1297,42 @@
       <c r="N18" s="2"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
       <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
+      <c r="U18" s="20"/>
       <c r="V18" s="5"/>
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
-      <c r="Z18" s="5"/>
+      <c r="Z18" s="20"/>
       <c r="AA18" s="5"/>
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
       <c r="AD18" s="5"/>
-      <c r="AE18" s="5"/>
+      <c r="AE18" s="20"/>
       <c r="AF18" s="5"/>
       <c r="AG18" s="5"/>
       <c r="AH18" s="5"/>
       <c r="AI18" s="5"/>
-      <c r="AJ18" s="5"/>
+      <c r="AJ18" s="20"/>
       <c r="AK18" s="5"/>
       <c r="AL18" s="5"/>
       <c r="AM18" s="5"/>
       <c r="AN18" s="5"/>
-      <c r="AO18" s="5"/>
+      <c r="AO18" s="20"/>
       <c r="AP18" s="5"/>
       <c r="AQ18" s="5"/>
       <c r="AR18" s="5"/>
       <c r="AS18" s="5"/>
-      <c r="AT18" s="5"/>
+      <c r="AT18" s="20"/>
       <c r="AU18" s="5"/>
-      <c r="AV18" s="5"/>
-      <c r="AW18" s="5"/>
-    </row>
-    <row r="19" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AV18" s="16"/>
+      <c r="AW18" s="16"/>
+      <c r="AX18" s="12"/>
+      <c r="AY18" s="12"/>
+    </row>
+    <row r="19" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1347,9 +1349,9 @@
       <c r="N19" s="8"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
       <c r="U19" s="5"/>
       <c r="V19" s="5"/>
       <c r="W19" s="5"/>
@@ -1372,15 +1374,17 @@
       <c r="AN19" s="5"/>
       <c r="AO19" s="5"/>
       <c r="AP19" s="5"/>
-      <c r="AQ19" s="5"/>
-      <c r="AR19" s="5"/>
-      <c r="AS19" s="5"/>
+      <c r="AQ19" s="16"/>
+      <c r="AR19" s="16"/>
+      <c r="AS19" s="16"/>
       <c r="AT19" s="5"/>
-      <c r="AU19" s="5"/>
-      <c r="AV19" s="5"/>
-      <c r="AW19" s="5"/>
-    </row>
-    <row r="20" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU19" s="16"/>
+      <c r="AV19" s="16"/>
+      <c r="AW19" s="16"/>
+      <c r="AX19" s="12"/>
+      <c r="AY19" s="12"/>
+    </row>
+    <row r="20" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1397,16 +1401,16 @@
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
       <c r="T20" s="5"/>
-      <c r="U20" s="16"/>
+      <c r="U20" s="5"/>
       <c r="V20" s="5"/>
       <c r="W20" s="16"/>
-      <c r="X20" s="5"/>
+      <c r="X20" s="16"/>
       <c r="Y20" s="16"/>
       <c r="Z20" s="5"/>
-      <c r="AA20" s="16"/>
+      <c r="AA20" s="5"/>
       <c r="AB20" s="5"/>
       <c r="AC20" s="5"/>
       <c r="AD20" s="5"/>
@@ -1418,19 +1422,21 @@
       <c r="AJ20" s="5"/>
       <c r="AK20" s="5"/>
       <c r="AL20" s="5"/>
-      <c r="AM20" s="16"/>
+      <c r="AM20" s="5"/>
       <c r="AN20" s="5"/>
-      <c r="AO20" s="16"/>
-      <c r="AP20" s="5"/>
+      <c r="AO20" s="5"/>
+      <c r="AP20" s="16"/>
       <c r="AQ20" s="16"/>
-      <c r="AR20" s="5"/>
+      <c r="AR20" s="16"/>
       <c r="AS20" s="16"/>
-      <c r="AT20" s="5"/>
+      <c r="AT20" s="16"/>
       <c r="AU20" s="5"/>
-      <c r="AV20" s="5"/>
+      <c r="AV20" s="16"/>
       <c r="AW20" s="16"/>
-    </row>
-    <row r="21" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AX20" s="12"/>
+      <c r="AY20" s="12"/>
+    </row>
+    <row r="21" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1447,40 +1453,42 @@
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
-      <c r="R21" s="5"/>
+      <c r="R21" s="20"/>
       <c r="S21" s="5"/>
-      <c r="T21" s="16"/>
+      <c r="T21" s="5"/>
       <c r="U21" s="5"/>
       <c r="V21" s="16"/>
-      <c r="W21" s="5"/>
+      <c r="W21" s="16"/>
       <c r="X21" s="16"/>
-      <c r="Y21" s="5"/>
+      <c r="Y21" s="16"/>
       <c r="Z21" s="16"/>
       <c r="AA21" s="5"/>
-      <c r="AB21" s="16"/>
+      <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
-      <c r="AF21" s="16"/>
+      <c r="AF21" s="5"/>
       <c r="AG21" s="5"/>
-      <c r="AH21" s="16"/>
+      <c r="AH21" s="5"/>
       <c r="AI21" s="5"/>
-      <c r="AJ21" s="16"/>
+      <c r="AJ21" s="5"/>
       <c r="AK21" s="5"/>
       <c r="AL21" s="5"/>
       <c r="AM21" s="5"/>
-      <c r="AN21" s="16"/>
+      <c r="AN21" s="5"/>
       <c r="AO21" s="5"/>
-      <c r="AP21" s="16"/>
-      <c r="AQ21" s="5"/>
+      <c r="AP21" s="5"/>
+      <c r="AQ21" s="16"/>
       <c r="AR21" s="16"/>
-      <c r="AS21" s="5"/>
+      <c r="AS21" s="16"/>
       <c r="AT21" s="5"/>
       <c r="AU21" s="5"/>
-      <c r="AV21" s="16"/>
-      <c r="AW21" s="5"/>
-    </row>
-    <row r="22" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AV21" s="5"/>
+      <c r="AW21" s="20"/>
+      <c r="AX21" s="12"/>
+      <c r="AY21" s="12"/>
+    </row>
+    <row r="22" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1497,24 +1505,24 @@
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
       <c r="V22" s="5"/>
-      <c r="W22" s="5"/>
-      <c r="X22" s="5"/>
-      <c r="Y22" s="5"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="16"/>
+      <c r="Y22" s="16"/>
       <c r="Z22" s="5"/>
-      <c r="AA22" s="16"/>
+      <c r="AA22" s="5"/>
       <c r="AB22" s="5"/>
       <c r="AC22" s="5"/>
-      <c r="AD22" s="5"/>
+      <c r="AD22" s="16"/>
       <c r="AE22" s="16"/>
-      <c r="AF22" s="5"/>
-      <c r="AG22" s="16"/>
+      <c r="AF22" s="16"/>
+      <c r="AG22" s="5"/>
       <c r="AH22" s="5"/>
-      <c r="AI22" s="16"/>
+      <c r="AI22" s="5"/>
       <c r="AJ22" s="5"/>
       <c r="AK22" s="5"/>
       <c r="AL22" s="5"/>
@@ -1522,15 +1530,15 @@
       <c r="AN22" s="5"/>
       <c r="AO22" s="5"/>
       <c r="AP22" s="5"/>
-      <c r="AQ22" s="16"/>
-      <c r="AR22" s="5"/>
-      <c r="AS22" s="16"/>
+      <c r="AQ22" s="5"/>
+      <c r="AR22" s="20"/>
+      <c r="AS22" s="5"/>
       <c r="AT22" s="5"/>
       <c r="AU22" s="5"/>
-      <c r="AV22" s="5"/>
+      <c r="AV22" s="16"/>
       <c r="AW22" s="16"/>
     </row>
-    <row r="23" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1547,22 +1555,22 @@
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
       <c r="P23" s="6"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
       <c r="T23" s="16"/>
       <c r="U23" s="5"/>
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
+      <c r="X23" s="20"/>
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
-      <c r="AB23" s="16"/>
-      <c r="AC23" s="5"/>
-      <c r="AD23" s="5"/>
-      <c r="AE23" s="5"/>
-      <c r="AF23" s="5"/>
-      <c r="AG23" s="5"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="16"/>
+      <c r="AD23" s="16"/>
+      <c r="AE23" s="16"/>
+      <c r="AF23" s="16"/>
+      <c r="AG23" s="16"/>
       <c r="AH23" s="5"/>
       <c r="AI23" s="5"/>
       <c r="AJ23" s="5"/>
@@ -1573,14 +1581,14 @@
       <c r="AO23" s="5"/>
       <c r="AP23" s="5"/>
       <c r="AQ23" s="5"/>
-      <c r="AR23" s="16"/>
+      <c r="AR23" s="5"/>
       <c r="AS23" s="5"/>
       <c r="AT23" s="5"/>
-      <c r="AU23" s="5"/>
+      <c r="AU23" s="16"/>
       <c r="AV23" s="16"/>
-      <c r="AW23" s="5"/>
-    </row>
-    <row r="24" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AW23" s="16"/>
+    </row>
+    <row r="24" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1597,27 +1605,27 @@
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="8"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
       <c r="T24" s="5"/>
       <c r="U24" s="5"/>
       <c r="V24" s="5"/>
-      <c r="W24" s="16"/>
-      <c r="X24" s="11"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
       <c r="AB24" s="5"/>
       <c r="AC24" s="5"/>
-      <c r="AD24" s="5"/>
-      <c r="AE24" s="5"/>
-      <c r="AF24" s="5"/>
-      <c r="AG24" s="5"/>
+      <c r="AD24" s="16"/>
+      <c r="AE24" s="16"/>
+      <c r="AF24" s="16"/>
+      <c r="AG24" s="11"/>
       <c r="AH24" s="5"/>
       <c r="AI24" s="5"/>
       <c r="AJ24" s="5"/>
       <c r="AK24" s="16"/>
-      <c r="AL24" s="5"/>
+      <c r="AL24" s="16"/>
       <c r="AM24" s="16"/>
       <c r="AN24" s="5"/>
       <c r="AO24" s="5"/>
@@ -1627,10 +1635,10 @@
       <c r="AS24" s="5"/>
       <c r="AT24" s="5"/>
       <c r="AU24" s="5"/>
-      <c r="AV24" s="5"/>
+      <c r="AV24" s="16"/>
       <c r="AW24" s="16"/>
     </row>
-    <row r="25" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1647,28 +1655,28 @@
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
-      <c r="R25" s="16"/>
+      <c r="R25" s="20"/>
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
       <c r="AA25" s="5"/>
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
       <c r="AD25" s="5"/>
-      <c r="AE25" s="5"/>
-      <c r="AF25" s="5"/>
-      <c r="AG25" s="5"/>
+      <c r="AE25" s="20"/>
+      <c r="AF25" s="11"/>
+      <c r="AG25" s="11"/>
       <c r="AH25" s="5"/>
       <c r="AI25" s="5"/>
       <c r="AJ25" s="16"/>
-      <c r="AK25" s="5"/>
+      <c r="AK25" s="16"/>
       <c r="AL25" s="16"/>
-      <c r="AM25" s="5"/>
+      <c r="AM25" s="16"/>
       <c r="AN25" s="16"/>
       <c r="AO25" s="5"/>
       <c r="AP25" s="5"/>
@@ -1677,10 +1685,10 @@
       <c r="AS25" s="5"/>
       <c r="AT25" s="5"/>
       <c r="AU25" s="5"/>
-      <c r="AV25" s="16"/>
-      <c r="AW25" s="5"/>
-    </row>
-    <row r="26" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AV25" s="5"/>
+      <c r="AW25" s="20"/>
+    </row>
+    <row r="26" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1697,40 +1705,40 @@
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
       <c r="T26" s="5"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="11"/>
-      <c r="Y26" s="11"/>
-      <c r="Z26" s="16"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
-      <c r="AD26" s="16"/>
-      <c r="AE26" s="5"/>
-      <c r="AF26" s="5"/>
-      <c r="AG26" s="5"/>
-      <c r="AH26" s="5"/>
+      <c r="AD26" s="11"/>
+      <c r="AE26" s="11"/>
+      <c r="AF26" s="11"/>
+      <c r="AG26" s="11"/>
+      <c r="AH26" s="11"/>
       <c r="AI26" s="5"/>
       <c r="AJ26" s="5"/>
-      <c r="AK26" s="5"/>
-      <c r="AL26" s="5"/>
+      <c r="AK26" s="16"/>
+      <c r="AL26" s="16"/>
       <c r="AM26" s="16"/>
       <c r="AN26" s="5"/>
       <c r="AO26" s="5"/>
       <c r="AP26" s="5"/>
-      <c r="AQ26" s="16"/>
+      <c r="AQ26" s="5"/>
       <c r="AR26" s="5"/>
-      <c r="AS26" s="16"/>
+      <c r="AS26" s="5"/>
       <c r="AT26" s="5"/>
       <c r="AU26" s="5"/>
-      <c r="AV26" s="5"/>
+      <c r="AV26" s="16"/>
       <c r="AW26" s="16"/>
     </row>
-    <row r="27" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="8"/>
       <c r="C27" s="6"/>
@@ -1747,40 +1755,40 @@
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="2"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
-      <c r="U27" s="16"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="16"/>
+      <c r="Y27" s="16"/>
+      <c r="Z27" s="16"/>
       <c r="AA27" s="5"/>
       <c r="AB27" s="5"/>
-      <c r="AC27" s="16"/>
+      <c r="AC27" s="5"/>
       <c r="AD27" s="5"/>
-      <c r="AE27" s="16"/>
-      <c r="AF27" s="5"/>
-      <c r="AG27" s="5"/>
-      <c r="AH27" s="5"/>
-      <c r="AI27" s="5"/>
+      <c r="AE27" s="11"/>
+      <c r="AF27" s="11"/>
+      <c r="AG27" s="11"/>
+      <c r="AH27" s="11"/>
+      <c r="AI27" s="11"/>
       <c r="AJ27" s="5"/>
       <c r="AK27" s="5"/>
-      <c r="AL27" s="5"/>
+      <c r="AL27" s="20"/>
       <c r="AM27" s="5"/>
-      <c r="AN27" s="16"/>
+      <c r="AN27" s="5"/>
       <c r="AO27" s="5"/>
       <c r="AP27" s="5"/>
       <c r="AQ27" s="5"/>
-      <c r="AR27" s="16"/>
+      <c r="AR27" s="5"/>
       <c r="AS27" s="5"/>
       <c r="AT27" s="5"/>
-      <c r="AU27" s="5"/>
+      <c r="AU27" s="16"/>
       <c r="AV27" s="16"/>
-      <c r="AW27" s="5"/>
-    </row>
-    <row r="28" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AW27" s="16"/>
+    </row>
+    <row r="28" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="8"/>
       <c r="C28" s="6"/>
@@ -1798,24 +1806,24 @@
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
       <c r="R28" s="16"/>
-      <c r="S28" s="5"/>
+      <c r="S28" s="16"/>
       <c r="T28" s="5"/>
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>
-      <c r="W28" s="11"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="5"/>
-      <c r="Z28" s="5"/>
-      <c r="AA28" s="5"/>
+      <c r="W28" s="16"/>
+      <c r="X28" s="16"/>
+      <c r="Y28" s="16"/>
+      <c r="Z28" s="16"/>
+      <c r="AA28" s="16"/>
       <c r="AB28" s="5"/>
       <c r="AC28" s="5"/>
       <c r="AD28" s="5"/>
       <c r="AE28" s="5"/>
-      <c r="AF28" s="5"/>
-      <c r="AG28" s="5"/>
-      <c r="AH28" s="16"/>
+      <c r="AF28" s="11"/>
+      <c r="AG28" s="11"/>
+      <c r="AH28" s="5"/>
       <c r="AI28" s="5"/>
-      <c r="AJ28" s="16"/>
+      <c r="AJ28" s="5"/>
       <c r="AK28" s="5"/>
       <c r="AL28" s="5"/>
       <c r="AM28" s="5"/>
@@ -1827,10 +1835,10 @@
       <c r="AS28" s="5"/>
       <c r="AT28" s="5"/>
       <c r="AU28" s="5"/>
-      <c r="AV28" s="5"/>
+      <c r="AV28" s="16"/>
       <c r="AW28" s="16"/>
     </row>
-    <row r="29" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="8"/>
@@ -1847,24 +1855,24 @@
       <c r="N29" s="8"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
-      <c r="R29" s="5"/>
+      <c r="R29" s="20"/>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
       <c r="U29" s="5"/>
       <c r="V29" s="5"/>
-      <c r="W29" s="11"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="16"/>
+      <c r="Y29" s="16"/>
+      <c r="Z29" s="16"/>
       <c r="AA29" s="5"/>
       <c r="AB29" s="5"/>
       <c r="AC29" s="5"/>
       <c r="AD29" s="5"/>
       <c r="AE29" s="5"/>
-      <c r="AF29" s="5"/>
-      <c r="AG29" s="16"/>
+      <c r="AF29" s="11"/>
+      <c r="AG29" s="5"/>
       <c r="AH29" s="5"/>
-      <c r="AI29" s="16"/>
+      <c r="AI29" s="5"/>
       <c r="AJ29" s="5"/>
       <c r="AK29" s="5"/>
       <c r="AL29" s="5"/>
@@ -1872,15 +1880,15 @@
       <c r="AN29" s="5"/>
       <c r="AO29" s="5"/>
       <c r="AP29" s="5"/>
-      <c r="AQ29" s="5"/>
-      <c r="AR29" s="5"/>
-      <c r="AS29" s="5"/>
+      <c r="AQ29" s="16"/>
+      <c r="AR29" s="16"/>
+      <c r="AS29" s="16"/>
       <c r="AT29" s="5"/>
       <c r="AU29" s="5"/>
-      <c r="AV29" s="16"/>
-      <c r="AW29" s="5"/>
-    </row>
-    <row r="30" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AV29" s="5"/>
+      <c r="AW29" s="20"/>
+    </row>
+    <row r="30" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="8"/>
@@ -1897,40 +1905,40 @@
       <c r="N30" s="5"/>
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+      <c r="T30" s="5"/>
       <c r="U30" s="5"/>
       <c r="V30" s="5"/>
       <c r="W30" s="5"/>
       <c r="X30" s="5"/>
-      <c r="Y30" s="5"/>
-      <c r="Z30" s="16"/>
+      <c r="Y30" s="20"/>
+      <c r="Z30" s="5"/>
       <c r="AA30" s="5"/>
       <c r="AB30" s="5"/>
-      <c r="AC30" s="16"/>
+      <c r="AC30" s="5"/>
       <c r="AD30" s="5"/>
       <c r="AE30" s="5"/>
       <c r="AF30" s="5"/>
       <c r="AG30" s="5"/>
-      <c r="AH30" s="16"/>
+      <c r="AH30" s="5"/>
       <c r="AI30" s="5"/>
-      <c r="AJ30" s="16"/>
+      <c r="AJ30" s="5"/>
       <c r="AK30" s="5"/>
       <c r="AL30" s="5"/>
-      <c r="AM30" s="16"/>
+      <c r="AM30" s="5"/>
       <c r="AN30" s="5"/>
       <c r="AO30" s="5"/>
-      <c r="AP30" s="5"/>
+      <c r="AP30" s="16"/>
       <c r="AQ30" s="16"/>
-      <c r="AR30" s="5"/>
+      <c r="AR30" s="16"/>
       <c r="AS30" s="16"/>
-      <c r="AT30" s="5"/>
+      <c r="AT30" s="16"/>
       <c r="AU30" s="5"/>
-      <c r="AV30" s="5"/>
+      <c r="AV30" s="16"/>
       <c r="AW30" s="16"/>
     </row>
-    <row r="31" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="8"/>
       <c r="C31" s="6"/>
@@ -1947,10 +1955,10 @@
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="16"/>
+      <c r="U31" s="5"/>
       <c r="V31" s="5"/>
       <c r="W31" s="5"/>
       <c r="X31" s="5"/>
@@ -1972,15 +1980,15 @@
       <c r="AN31" s="5"/>
       <c r="AO31" s="5"/>
       <c r="AP31" s="5"/>
-      <c r="AQ31" s="5"/>
+      <c r="AQ31" s="16"/>
       <c r="AR31" s="16"/>
-      <c r="AS31" s="5"/>
+      <c r="AS31" s="16"/>
       <c r="AT31" s="5"/>
-      <c r="AU31" s="5"/>
+      <c r="AU31" s="16"/>
       <c r="AV31" s="16"/>
-      <c r="AW31" s="5"/>
-    </row>
-    <row r="32" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AW31" s="16"/>
+    </row>
+    <row r="32" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
@@ -1997,8 +2005,8 @@
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="16"/>
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
       <c r="V32" s="5"/>
@@ -2023,48 +2031,48 @@
       <c r="AO32" s="5"/>
       <c r="AP32" s="5"/>
       <c r="AQ32" s="5"/>
-      <c r="AR32" s="5"/>
+      <c r="AR32" s="20"/>
       <c r="AS32" s="5"/>
       <c r="AT32" s="5"/>
       <c r="AU32" s="5"/>
-      <c r="AV32" s="5"/>
-      <c r="AW32" s="5"/>
+      <c r="AV32" s="16"/>
+      <c r="AW32" s="16"/>
     </row>
     <row r="33" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
-      <c r="R33" s="5"/>
+      <c r="R33" s="20"/>
       <c r="S33" s="5"/>
-      <c r="T33" s="5"/>
-      <c r="U33" s="5"/>
-      <c r="V33" s="5"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
       <c r="W33" s="5"/>
       <c r="X33" s="5"/>
-      <c r="Y33" s="5"/>
-      <c r="Z33" s="5"/>
-      <c r="AA33" s="5"/>
+      <c r="Y33" s="16"/>
+      <c r="Z33" s="16"/>
+      <c r="AA33" s="16"/>
       <c r="AB33" s="5"/>
       <c r="AC33" s="5"/>
-      <c r="AD33" s="5"/>
-      <c r="AE33" s="5"/>
-      <c r="AF33" s="5"/>
+      <c r="AD33" s="16"/>
+      <c r="AE33" s="16"/>
+      <c r="AF33" s="16"/>
       <c r="AG33" s="5"/>
       <c r="AH33" s="5"/>
-      <c r="AI33" s="5"/>
-      <c r="AJ33" s="5"/>
-      <c r="AK33" s="5"/>
+      <c r="AI33" s="16"/>
+      <c r="AJ33" s="16"/>
+      <c r="AK33" s="16"/>
       <c r="AL33" s="5"/>
       <c r="AM33" s="5"/>
-      <c r="AN33" s="5"/>
-      <c r="AO33" s="5"/>
-      <c r="AP33" s="5"/>
+      <c r="AN33" s="16"/>
+      <c r="AO33" s="16"/>
+      <c r="AP33" s="16"/>
       <c r="AQ33" s="5"/>
       <c r="AR33" s="5"/>
-      <c r="AS33" s="5"/>
-      <c r="AT33" s="5"/>
-      <c r="AU33" s="5"/>
+      <c r="AS33" s="16"/>
+      <c r="AT33" s="16"/>
+      <c r="AU33" s="16"/>
       <c r="AV33" s="5"/>
-      <c r="AW33" s="5"/>
+      <c r="AW33" s="20"/>
     </row>
     <row r="34" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
@@ -2083,6 +2091,36 @@
       <c r="N34" s="11"/>
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="12"/>
+      <c r="U34" s="12"/>
+      <c r="V34" s="12"/>
+      <c r="W34" s="12"/>
+      <c r="X34" s="12"/>
+      <c r="Y34" s="12"/>
+      <c r="Z34" s="12"/>
+      <c r="AA34" s="12"/>
+      <c r="AB34" s="12"/>
+      <c r="AC34" s="12"/>
+      <c r="AD34" s="12"/>
+      <c r="AE34" s="12"/>
+      <c r="AF34" s="12"/>
+      <c r="AG34" s="12"/>
+      <c r="AH34" s="12"/>
+      <c r="AI34" s="12"/>
+      <c r="AJ34" s="12"/>
+      <c r="AK34" s="12"/>
+      <c r="AL34" s="12"/>
+      <c r="AM34" s="12"/>
+      <c r="AN34" s="12"/>
+      <c r="AO34" s="12"/>
+      <c r="AP34" s="12"/>
+      <c r="AQ34" s="12"/>
+      <c r="AR34" s="12"/>
+      <c r="AS34" s="12"/>
+      <c r="AT34" s="12"/>
+      <c r="AU34" s="12"/>
     </row>
     <row r="35" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
@@ -2101,6 +2139,36 @@
       <c r="N35" s="11"/>
       <c r="O35" s="11"/>
       <c r="P35" s="11"/>
+      <c r="R35" s="12"/>
+      <c r="S35" s="12"/>
+      <c r="T35" s="12"/>
+      <c r="U35" s="12"/>
+      <c r="V35" s="12"/>
+      <c r="W35" s="12"/>
+      <c r="X35" s="12"/>
+      <c r="Y35" s="12"/>
+      <c r="Z35" s="12"/>
+      <c r="AA35" s="12"/>
+      <c r="AB35" s="12"/>
+      <c r="AC35" s="12"/>
+      <c r="AD35" s="12"/>
+      <c r="AE35" s="12"/>
+      <c r="AF35" s="12"/>
+      <c r="AG35" s="12"/>
+      <c r="AH35" s="12"/>
+      <c r="AI35" s="12"/>
+      <c r="AJ35" s="12"/>
+      <c r="AK35" s="12"/>
+      <c r="AL35" s="12"/>
+      <c r="AM35" s="12"/>
+      <c r="AN35" s="12"/>
+      <c r="AO35" s="12"/>
+      <c r="AP35" s="12"/>
+      <c r="AQ35" s="12"/>
+      <c r="AR35" s="12"/>
+      <c r="AS35" s="12"/>
+      <c r="AT35" s="12"/>
+      <c r="AU35" s="12"/>
     </row>
     <row r="36" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
@@ -2119,6 +2187,36 @@
       <c r="N36" s="11"/>
       <c r="O36" s="11"/>
       <c r="P36" s="11"/>
+      <c r="R36" s="12"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="12"/>
+      <c r="U36" s="12"/>
+      <c r="V36" s="12"/>
+      <c r="W36" s="12"/>
+      <c r="X36" s="12"/>
+      <c r="Y36" s="12"/>
+      <c r="Z36" s="12"/>
+      <c r="AA36" s="12"/>
+      <c r="AB36" s="12"/>
+      <c r="AC36" s="12"/>
+      <c r="AD36" s="12"/>
+      <c r="AE36" s="12"/>
+      <c r="AF36" s="12"/>
+      <c r="AG36" s="12"/>
+      <c r="AH36" s="12"/>
+      <c r="AI36" s="12"/>
+      <c r="AJ36" s="12"/>
+      <c r="AK36" s="12"/>
+      <c r="AL36" s="12"/>
+      <c r="AM36" s="12"/>
+      <c r="AN36" s="12"/>
+      <c r="AO36" s="12"/>
+      <c r="AP36" s="12"/>
+      <c r="AQ36" s="12"/>
+      <c r="AR36" s="12"/>
+      <c r="AS36" s="12"/>
+      <c r="AT36" s="12"/>
+      <c r="AU36" s="12"/>
     </row>
     <row r="37" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>

</xml_diff>

<commit_message>
added tree, fixed map, help
</commit_message>
<xml_diff>
--- a/sprites/land/mapDesign.xlsx
+++ b/sprites/land/mapDesign.xlsx
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD29" sqref="AD29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added a few corners
</commit_message>
<xml_diff>
--- a/sprites/land/mapDesign.xlsx
+++ b/sprites/land/mapDesign.xlsx
@@ -21,10 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -472,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -736,7 +732,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="6"/>
@@ -784,7 +780,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="6"/>
@@ -831,7 +827,7 @@
     <row r="8" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -841,7 +837,7 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="8"/>
-      <c r="M8" s="5"/>
+      <c r="M8" s="8"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
@@ -880,7 +876,7 @@
     </row>
     <row r="9" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -929,7 +925,7 @@
       <c r="AW9" s="9"/>
     </row>
     <row r="10" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -940,7 +936,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="5"/>
+      <c r="L10" s="8"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -990,7 +986,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="5"/>
+      <c r="L11" s="8"/>
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1190,7 +1186,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
-      <c r="L15" s="5"/>
+      <c r="L15" s="8"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -1229,7 +1225,7 @@
       <c r="AW15" s="4"/>
     </row>
     <row r="16" spans="1:49" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1240,7 +1236,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="5"/>
+      <c r="L16" s="8"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
@@ -1280,7 +1276,7 @@
     </row>
     <row r="17" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="6"/>
@@ -1290,7 +1286,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="5"/>
+      <c r="L17" s="8"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -1300,7 +1296,7 @@
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="6"/>
@@ -1354,7 +1350,7 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="6"/>
@@ -1405,7 +1401,7 @@
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="6"/>
@@ -1455,7 +1451,7 @@
     <row r="21" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="6"/>
@@ -1505,7 +1501,7 @@
       <c r="AY21" s="12"/>
     </row>
     <row r="22" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="6"/>
@@ -1564,7 +1560,7 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="5"/>
+      <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
@@ -1614,12 +1610,12 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="5"/>
+      <c r="J24" s="8"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
+      <c r="O24" s="8"/>
       <c r="P24" s="8"/>
       <c r="R24" s="16"/>
       <c r="S24" s="16"/>
@@ -1665,7 +1661,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="8"/>
-      <c r="K25" s="5"/>
+      <c r="K25" s="8"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
@@ -1716,7 +1712,7 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="8"/>
-      <c r="L26" s="5"/>
+      <c r="L26" s="8"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
@@ -1755,7 +1751,7 @@
       <c r="AW26" s="16"/>
     </row>
     <row r="27" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -1767,7 +1763,7 @@
       <c r="J27" s="8"/>
       <c r="K27" s="6"/>
       <c r="L27" s="8"/>
-      <c r="M27" s="5"/>
+      <c r="M27" s="8"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="2"/>
@@ -1856,7 +1852,7 @@
     </row>
     <row r="29" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="6"/>
       <c r="E29" s="2"/>
@@ -1867,7 +1863,7 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="8"/>
-      <c r="M29" s="5"/>
+      <c r="M29" s="8"/>
       <c r="N29" s="8"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -1906,7 +1902,7 @@
     </row>
     <row r="30" spans="1:51" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="6"/>
       <c r="E30" s="1"/>
@@ -1916,7 +1912,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
-      <c r="L30" s="5"/>
+      <c r="L30" s="8"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="8"/>
@@ -1963,7 +1959,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
-      <c r="I31" s="5"/>
+      <c r="I31" s="8"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
@@ -2011,7 +2007,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
-      <c r="G32" s="5"/>
+      <c r="G32" s="8"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>

</xml_diff>